<commit_message>
Trimmed all blank rows/columns
arcpy was processing indefinitely (or at least impractically long) when reading `District Monitoring.xlsx`. Deleted all columns and rows that looked blank, to ensure that Excel/ArcGIS didn't consider them valid "table" cells that just happened to be empty. Fixed issue.
</commit_message>
<xml_diff>
--- a/data/District Monitoring.xlsx
+++ b/data/District Monitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k_price\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\manniongeo\projects\nwfwmd\2015-01-13_gis_support\github\Hydrologic-Monitoring-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725DE993-94B5-4737-8496-89F80F32D020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F699AE46-8E94-4803-BC39-1E4B02654E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive Monitoring" sheetId="3" r:id="rId1"/>
@@ -5023,7 +5023,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -5041,7 +5041,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -5658,10 +5658,10 @@
   <dimension ref="A1:AN459"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C445" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F465" sqref="F465"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5706,7 +5706,6 @@
     <col min="38" max="38" width="14.85546875" customWidth="1"/>
     <col min="39" max="39" width="15.140625" customWidth="1"/>
     <col min="40" max="40" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" s="6" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -40701,23 +40700,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f" xsi:nil="true"/>
-    <SharedWithUsers xmlns="5bc6a959-17f5-4671-a856-850152dcb308">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <uegw xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="5bc6a959-17f5-4671-a856-850152dcb308" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40976,21 +40964,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f" xsi:nil="true"/>
+    <SharedWithUsers xmlns="5bc6a959-17f5-4671-a856-850152dcb308">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <uegw xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5bc6a959-17f5-4671-a856-850152dcb308" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F5B2541-43D0-49A1-8374-BB26BE387144}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{282EF33A-C6D9-498B-9EDB-B03D7B5BFEE6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d3d772d5-8785-49ba-8d87-9ce83f8f842f"/>
-    <ds:schemaRef ds:uri="5bc6a959-17f5-4671-a856-850152dcb308"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -41015,9 +41011,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{282EF33A-C6D9-498B-9EDB-B03D7B5BFEE6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F5B2541-43D0-49A1-8374-BB26BE387144}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d3d772d5-8785-49ba-8d87-9ce83f8f842f"/>
+    <ds:schemaRef ds:uri="5bc6a959-17f5-4671-a856-850152dcb308"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Test site 222222 with TB SN
</commit_message>
<xml_diff>
--- a/data/District Monitoring.xlsx
+++ b/data/District Monitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\rmd1\users\k_price\Survey123_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE277CE5-55C1-4DAE-A136-C17F5A9AD2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D394305B-0A04-4EEA-A844-948843F8AE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5565" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="165" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comprehensive Monitoring" sheetId="3" r:id="rId1"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5051" uniqueCount="1041">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5052" uniqueCount="1041">
   <si>
     <t>Station ID</t>
   </si>
@@ -6265,10 +6265,10 @@
   <dimension ref="A1:AS475"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K454" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AI454" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q471" sqref="Q471"/>
+      <selection pane="bottomRight" activeCell="AJ471" sqref="AJ471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43065,8 +43065,12 @@
       <c r="AF471" s="89"/>
       <c r="AG471" s="89"/>
       <c r="AH471" s="89"/>
-      <c r="AI471" s="89"/>
-      <c r="AJ471" s="89"/>
+      <c r="AI471" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ471" s="89">
+        <v>222222</v>
+      </c>
       <c r="AK471" s="89"/>
       <c r="AL471" s="89"/>
       <c r="AM471" s="89"/>
@@ -43096,46 +43100,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f" xsi:nil="true"/>
-    <SharedWithUsers xmlns="5bc6a959-17f5-4671-a856-850152dcb308">
-      <UserInfo>
-        <DisplayName>Kathleen Coates</DisplayName>
-        <AccountId>43</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Katie Price</DisplayName>
-        <AccountId>61</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Tony Countryman</DisplayName>
-        <AccountId>46</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Paul Thurman</DisplayName>
-        <AccountId>45</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Steve Costa</DisplayName>
-        <AccountId>56</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <uegw xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="5bc6a959-17f5-4671-a856-850152dcb308" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E53827B1A17CD040A82F4CB6493BE107" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd232c0e9954280ca5703afa7e5a7b0c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3d772d5-8785-49ba-8d87-9ce83f8f842f" xmlns:ns3="5bc6a959-17f5-4671-a856-850152dcb308" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="244dc119bbf5629589ee693515a62b2a" ns2:_="" ns3:_="">
     <xsd:import namespace="d3d772d5-8785-49ba-8d87-9ce83f8f842f"/>
@@ -43402,6 +43366,46 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f" xsi:nil="true"/>
+    <SharedWithUsers xmlns="5bc6a959-17f5-4671-a856-850152dcb308">
+      <UserInfo>
+        <DisplayName>Kathleen Coates</DisplayName>
+        <AccountId>43</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Katie Price</DisplayName>
+        <AccountId>61</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Tony Countryman</DisplayName>
+        <AccountId>46</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Paul Thurman</DisplayName>
+        <AccountId>45</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Steve Costa</DisplayName>
+        <AccountId>56</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <uegw xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3d772d5-8785-49ba-8d87-9ce83f8f842f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5bc6a959-17f5-4671-a856-850152dcb308" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -43412,17 +43416,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F5B2541-43D0-49A1-8374-BB26BE387144}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d3d772d5-8785-49ba-8d87-9ce83f8f842f"/>
-    <ds:schemaRef ds:uri="5bc6a959-17f5-4671-a856-850152dcb308"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7826E5-3E1C-48F1-A433-5F771AF96D89}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43441,6 +43434,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F5B2541-43D0-49A1-8374-BB26BE387144}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d3d772d5-8785-49ba-8d87-9ce83f8f842f"/>
+    <ds:schemaRef ds:uri="5bc6a959-17f5-4671-a856-850152dcb308"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{282EF33A-C6D9-498B-9EDB-B03D7B5BFEE6}">
   <ds:schemaRefs>

</xml_diff>